<commit_message>
TS Jatai Raja Changes 02/09/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Input Raja.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Input Raja.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3344" uniqueCount="1987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="1995">
   <si>
     <t>4.5.1.1</t>
   </si>
@@ -6030,6 +6030,30 @@
   </si>
   <si>
     <t xml:space="preserve">mada#H </t>
+  </si>
+  <si>
+    <t>6.1.4.6</t>
+  </si>
+  <si>
+    <t>5.2.1.3</t>
+  </si>
+  <si>
+    <t>apa#</t>
+  </si>
+  <si>
+    <t>iqtaq</t>
+  </si>
+  <si>
+    <t>1.6.3.1</t>
+  </si>
+  <si>
+    <t>iqmAn</t>
+  </si>
+  <si>
+    <t>4.6.6.1</t>
+  </si>
+  <si>
+    <t>iqvaq</t>
   </si>
 </sst>
 </file>
@@ -6214,7 +6238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6414,6 +6438,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6697,9 +6724,9 @@
   <dimension ref="A1:AC990"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A782" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A822" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S792" sqref="S792"/>
+      <selection pane="bottomLeft" activeCell="P829" sqref="P829"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -37429,11 +37456,22 @@
     </row>
     <row r="813" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I813" s="68"/>
-      <c r="J813" s="68"/>
-      <c r="K813" s="68"/>
-      <c r="L813" s="71"/>
-      <c r="M813" s="71"/>
-      <c r="N813" s="68"/>
+      <c r="J813" s="75" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K813" s="8">
+        <f t="shared" ref="K813" si="428">+K812+1</f>
+        <v>733</v>
+      </c>
+      <c r="L813" s="13">
+        <v>1</v>
+      </c>
+      <c r="M813" s="13">
+        <v>1</v>
+      </c>
+      <c r="N813" s="75" t="s">
+        <v>106</v>
+      </c>
       <c r="O813" s="14"/>
       <c r="P813" s="15"/>
       <c r="Q813" s="15"/>
@@ -37448,11 +37486,24 @@
     </row>
     <row r="814" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I814" s="68"/>
-      <c r="J814" s="68"/>
-      <c r="K814" s="68"/>
-      <c r="L814" s="71"/>
-      <c r="M814" s="71"/>
-      <c r="N814" s="68"/>
+      <c r="J814" s="75" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K814" s="8">
+        <f t="shared" ref="K814" si="429">+K813+1</f>
+        <v>734</v>
+      </c>
+      <c r="L814" s="13">
+        <f>+L813+1</f>
+        <v>2</v>
+      </c>
+      <c r="M814" s="13">
+        <f>+M813+1</f>
+        <v>2</v>
+      </c>
+      <c r="N814" s="75" t="s">
+        <v>341</v>
+      </c>
       <c r="O814" s="14"/>
       <c r="P814" s="15"/>
       <c r="Q814" s="15"/>
@@ -37467,13 +37518,28 @@
     </row>
     <row r="815" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I815" s="68"/>
-      <c r="J815" s="68"/>
-      <c r="K815" s="68"/>
-      <c r="L815" s="71"/>
-      <c r="M815" s="71"/>
-      <c r="N815" s="68"/>
+      <c r="J815" s="75" t="s">
+        <v>1987</v>
+      </c>
+      <c r="K815" s="8">
+        <f t="shared" ref="K815:M818" si="430">+K814+1</f>
+        <v>735</v>
+      </c>
+      <c r="L815" s="13">
+        <f t="shared" ref="L815:M815" si="431">+L814+1</f>
+        <v>3</v>
+      </c>
+      <c r="M815" s="13">
+        <f t="shared" si="431"/>
+        <v>3</v>
+      </c>
+      <c r="N815" s="75" t="s">
+        <v>342</v>
+      </c>
       <c r="O815" s="14"/>
-      <c r="P815" s="15"/>
+      <c r="P815" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="Q815" s="15"/>
       <c r="R815" s="15"/>
       <c r="S815" s="15"/>
@@ -37486,11 +37552,22 @@
     </row>
     <row r="816" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I816" s="68"/>
-      <c r="J816" s="68"/>
-      <c r="K816" s="68"/>
-      <c r="L816" s="71"/>
-      <c r="M816" s="71"/>
-      <c r="N816" s="68"/>
+      <c r="J816" s="75" t="s">
+        <v>1988</v>
+      </c>
+      <c r="K816" s="8">
+        <f t="shared" si="430"/>
+        <v>736</v>
+      </c>
+      <c r="L816" s="13">
+        <v>1</v>
+      </c>
+      <c r="M816" s="13">
+        <v>1</v>
+      </c>
+      <c r="N816" s="75" t="s">
+        <v>1989</v>
+      </c>
       <c r="O816" s="14"/>
       <c r="P816" s="15"/>
       <c r="Q816" s="15"/>
@@ -37505,11 +37582,24 @@
     </row>
     <row r="817" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I817" s="68"/>
-      <c r="J817" s="68"/>
-      <c r="K817" s="68"/>
-      <c r="L817" s="71"/>
-      <c r="M817" s="71"/>
-      <c r="N817" s="68"/>
+      <c r="J817" s="75" t="s">
+        <v>1988</v>
+      </c>
+      <c r="K817" s="8">
+        <f t="shared" si="430"/>
+        <v>737</v>
+      </c>
+      <c r="L817" s="13">
+        <f>+L816+1</f>
+        <v>2</v>
+      </c>
+      <c r="M817" s="13">
+        <f>+M816+1</f>
+        <v>2</v>
+      </c>
+      <c r="N817" s="75" t="s">
+        <v>1990</v>
+      </c>
       <c r="O817" s="14"/>
       <c r="P817" s="15"/>
       <c r="Q817" s="15"/>
@@ -37524,13 +37614,28 @@
     </row>
     <row r="818" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I818" s="68"/>
-      <c r="J818" s="68"/>
-      <c r="K818" s="68"/>
-      <c r="L818" s="71"/>
-      <c r="M818" s="71"/>
-      <c r="N818" s="68"/>
+      <c r="J818" s="75" t="s">
+        <v>1988</v>
+      </c>
+      <c r="K818" s="8">
+        <f t="shared" si="430"/>
+        <v>738</v>
+      </c>
+      <c r="L818" s="13">
+        <f t="shared" si="430"/>
+        <v>3</v>
+      </c>
+      <c r="M818" s="13">
+        <f t="shared" si="430"/>
+        <v>3</v>
+      </c>
+      <c r="N818" s="75" t="s">
+        <v>341</v>
+      </c>
       <c r="O818" s="14"/>
-      <c r="P818" s="15"/>
+      <c r="P818" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="Q818" s="15"/>
       <c r="R818" s="15"/>
       <c r="S818" s="15"/>
@@ -37543,11 +37648,22 @@
     </row>
     <row r="819" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I819" s="68"/>
-      <c r="J819" s="68"/>
-      <c r="K819" s="68"/>
-      <c r="L819" s="71"/>
-      <c r="M819" s="71"/>
-      <c r="N819" s="68"/>
+      <c r="J819" s="75" t="s">
+        <v>1991</v>
+      </c>
+      <c r="K819" s="8">
+        <f t="shared" ref="K819" si="432">+K818+1</f>
+        <v>739</v>
+      </c>
+      <c r="L819" s="13">
+        <v>1</v>
+      </c>
+      <c r="M819" s="13">
+        <v>1</v>
+      </c>
+      <c r="N819" s="75" t="s">
+        <v>106</v>
+      </c>
       <c r="O819" s="14"/>
       <c r="P819" s="15"/>
       <c r="Q819" s="15"/>
@@ -37562,11 +37678,24 @@
     </row>
     <row r="820" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I820" s="68"/>
-      <c r="J820" s="68"/>
-      <c r="K820" s="68"/>
-      <c r="L820" s="71"/>
-      <c r="M820" s="71"/>
-      <c r="N820" s="68"/>
+      <c r="J820" s="75" t="s">
+        <v>1991</v>
+      </c>
+      <c r="K820" s="8">
+        <f t="shared" ref="K820" si="433">+K819+1</f>
+        <v>740</v>
+      </c>
+      <c r="L820" s="13">
+        <f>+L819+1</f>
+        <v>2</v>
+      </c>
+      <c r="M820" s="13">
+        <f>+M819+1</f>
+        <v>2</v>
+      </c>
+      <c r="N820" s="75" t="s">
+        <v>1828</v>
+      </c>
       <c r="O820" s="14"/>
       <c r="P820" s="15"/>
       <c r="Q820" s="15"/>
@@ -37581,13 +37710,28 @@
     </row>
     <row r="821" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I821" s="68"/>
-      <c r="J821" s="68"/>
-      <c r="K821" s="68"/>
-      <c r="L821" s="71"/>
-      <c r="M821" s="71"/>
-      <c r="N821" s="68"/>
+      <c r="J821" s="75" t="s">
+        <v>1991</v>
+      </c>
+      <c r="K821" s="8">
+        <f t="shared" ref="K821:M821" si="434">+K820+1</f>
+        <v>741</v>
+      </c>
+      <c r="L821" s="13">
+        <f t="shared" si="434"/>
+        <v>3</v>
+      </c>
+      <c r="M821" s="13">
+        <f t="shared" si="434"/>
+        <v>3</v>
+      </c>
+      <c r="N821" s="75" t="s">
+        <v>1992</v>
+      </c>
       <c r="O821" s="14"/>
-      <c r="P821" s="15"/>
+      <c r="P821" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="Q821" s="15"/>
       <c r="R821" s="15"/>
       <c r="S821" s="15"/>
@@ -37600,11 +37744,22 @@
     </row>
     <row r="822" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I822" s="68"/>
-      <c r="J822" s="68"/>
-      <c r="K822" s="68"/>
-      <c r="L822" s="71"/>
-      <c r="M822" s="71"/>
-      <c r="N822" s="68"/>
+      <c r="J822" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="K822" s="8">
+        <f t="shared" ref="K822" si="435">+K821+1</f>
+        <v>742</v>
+      </c>
+      <c r="L822" s="13">
+        <v>1</v>
+      </c>
+      <c r="M822" s="13">
+        <v>1</v>
+      </c>
+      <c r="N822" s="75" t="s">
+        <v>341</v>
+      </c>
       <c r="O822" s="14"/>
       <c r="P822" s="15"/>
       <c r="Q822" s="15"/>
@@ -37619,11 +37774,24 @@
     </row>
     <row r="823" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I823" s="68"/>
-      <c r="J823" s="68"/>
-      <c r="K823" s="68"/>
-      <c r="L823" s="71"/>
-      <c r="M823" s="71"/>
-      <c r="N823" s="68"/>
+      <c r="J823" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="K823" s="8">
+        <f t="shared" ref="K823" si="436">+K822+1</f>
+        <v>743</v>
+      </c>
+      <c r="L823" s="13">
+        <f>+L822+1</f>
+        <v>2</v>
+      </c>
+      <c r="M823" s="13">
+        <f>+M822+1</f>
+        <v>2</v>
+      </c>
+      <c r="N823" s="75" t="s">
+        <v>342</v>
+      </c>
       <c r="O823" s="14"/>
       <c r="P823" s="15"/>
       <c r="Q823" s="15"/>
@@ -37638,11 +37806,24 @@
     </row>
     <row r="824" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I824" s="68"/>
-      <c r="J824" s="68"/>
-      <c r="K824" s="68"/>
-      <c r="L824" s="71"/>
-      <c r="M824" s="71"/>
-      <c r="N824" s="68"/>
+      <c r="J824" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="K824" s="8">
+        <f t="shared" ref="K824:L825" si="437">+K823+1</f>
+        <v>744</v>
+      </c>
+      <c r="L824" s="13">
+        <f t="shared" si="437"/>
+        <v>3</v>
+      </c>
+      <c r="M824" s="13">
+        <f t="shared" ref="M824:M825" si="438">+M823+1</f>
+        <v>3</v>
+      </c>
+      <c r="N824" s="75" t="s">
+        <v>106</v>
+      </c>
       <c r="O824" s="14"/>
       <c r="P824" s="15"/>
       <c r="Q824" s="15"/>
@@ -37657,13 +37838,28 @@
     </row>
     <row r="825" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I825" s="68"/>
-      <c r="J825" s="68"/>
-      <c r="K825" s="68"/>
-      <c r="L825" s="71"/>
-      <c r="M825" s="71"/>
-      <c r="N825" s="68"/>
+      <c r="J825" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="K825" s="8">
+        <f t="shared" ref="K825:M828" si="439">+K824+1</f>
+        <v>745</v>
+      </c>
+      <c r="L825" s="13">
+        <f t="shared" si="437"/>
+        <v>4</v>
+      </c>
+      <c r="M825" s="13">
+        <f t="shared" si="438"/>
+        <v>4</v>
+      </c>
+      <c r="N825" s="75" t="s">
+        <v>774</v>
+      </c>
       <c r="O825" s="14"/>
-      <c r="P825" s="15"/>
+      <c r="P825" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="Q825" s="15"/>
       <c r="R825" s="15"/>
       <c r="S825" s="15"/>
@@ -37676,11 +37872,22 @@
     </row>
     <row r="826" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I826" s="68"/>
-      <c r="J826" s="68"/>
-      <c r="K826" s="68"/>
-      <c r="L826" s="71"/>
-      <c r="M826" s="71"/>
-      <c r="N826" s="68"/>
+      <c r="J826" s="75" t="s">
+        <v>1993</v>
+      </c>
+      <c r="K826" s="8">
+        <f t="shared" si="439"/>
+        <v>746</v>
+      </c>
+      <c r="L826" s="13">
+        <v>1</v>
+      </c>
+      <c r="M826" s="13">
+        <v>1</v>
+      </c>
+      <c r="N826" s="75" t="s">
+        <v>1994</v>
+      </c>
       <c r="O826" s="14"/>
       <c r="P826" s="15"/>
       <c r="Q826" s="15"/>
@@ -37695,11 +37902,24 @@
     </row>
     <row r="827" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I827" s="68"/>
-      <c r="J827" s="68"/>
-      <c r="K827" s="68"/>
-      <c r="L827" s="71"/>
-      <c r="M827" s="71"/>
-      <c r="N827" s="68"/>
+      <c r="J827" s="75" t="s">
+        <v>1993</v>
+      </c>
+      <c r="K827" s="8">
+        <f t="shared" si="439"/>
+        <v>747</v>
+      </c>
+      <c r="L827" s="13">
+        <f>+L826+1</f>
+        <v>2</v>
+      </c>
+      <c r="M827" s="13">
+        <f>+M826+1</f>
+        <v>2</v>
+      </c>
+      <c r="N827" s="75" t="s">
+        <v>341</v>
+      </c>
       <c r="O827" s="14"/>
       <c r="P827" s="15"/>
       <c r="Q827" s="15"/>
@@ -37714,13 +37934,28 @@
     </row>
     <row r="828" spans="9:25" x14ac:dyDescent="0.25">
       <c r="I828" s="68"/>
-      <c r="J828" s="68"/>
-      <c r="K828" s="68"/>
-      <c r="L828" s="71"/>
-      <c r="M828" s="71"/>
-      <c r="N828" s="68"/>
+      <c r="J828" s="75" t="s">
+        <v>1993</v>
+      </c>
+      <c r="K828" s="8">
+        <f t="shared" si="439"/>
+        <v>748</v>
+      </c>
+      <c r="L828" s="13">
+        <f t="shared" si="439"/>
+        <v>3</v>
+      </c>
+      <c r="M828" s="13">
+        <f t="shared" si="439"/>
+        <v>3</v>
+      </c>
+      <c r="N828" s="75" t="s">
+        <v>106</v>
+      </c>
       <c r="O828" s="14"/>
-      <c r="P828" s="15"/>
+      <c r="P828" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="Q828" s="15"/>
       <c r="R828" s="15"/>
       <c r="S828" s="15"/>

</xml_diff>